<commit_message>
Plan de pruebas de integración
Le agregué las pruebas que faltaban respecto al plan. Falta llenar los
pasos a realizar para cada una de las pruebas
</commit_message>
<xml_diff>
--- a/Documentacion/PPI_Nutrición_Plan_Pruebas_Integracion.xlsx
+++ b/Documentacion/PPI_Nutrición_Plan_Pruebas_Integracion.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Hoja de Control'!$B$2:$F$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Pruebas de Integración'!$A$1:$G$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Pruebas de Integración'!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="95">
   <si>
     <t>&lt;Nombre Proyecto&gt;</t>
   </si>
@@ -526,13 +526,58 @@
   <si>
     <t>Tener datos base agregados en la base de datos de nutrición comunitaria</t>
   </si>
+  <si>
+    <t>PI9</t>
+  </si>
+  <si>
+    <t>PI10</t>
+  </si>
+  <si>
+    <t>PI11</t>
+  </si>
+  <si>
+    <t>PI12</t>
+  </si>
+  <si>
+    <t>Login - Página principal de la aplicación web</t>
+  </si>
+  <si>
+    <t>Ingresar un usuario y contraseña que se hayan registrado previamente</t>
+  </si>
+  <si>
+    <t>Después de pasar el filtro de inicio de sesión de la aplicación web se debe mostrar la página principal de la misma</t>
+  </si>
+  <si>
+    <t>El usuario debe estar dado de alta en la base de datos de pacientes</t>
+  </si>
+  <si>
+    <t>Login de la aplicación móvil (primera vez) - aviso de privacidad</t>
+  </si>
+  <si>
+    <t>Aviso de privacidad - pantalla principal</t>
+  </si>
+  <si>
+    <t>Después de aceptar los términos y condiciones del aviso de privacidad, el usuario podrá entrar a la pantalla pricipal de la aplicación móvil</t>
+  </si>
+  <si>
+    <t>Después de iniciar sesión en la aplicación móvil por primera vez deberá presentarse al usuario un aviso de privacidad</t>
+  </si>
+  <si>
+    <t>En caso de no aceptar los terminos el paciente no podrá ingresar a la aplicación</t>
+  </si>
+  <si>
+    <t>Login de la aplicación móvil - pantalla principal</t>
+  </si>
+  <si>
+    <t>Luego de iniciar sesión se presentará al usuario la pantalla principal de la aplicación</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€]"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1620,7 +1665,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1714,39 +1759,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="26" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1775,84 +1787,117 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="25" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="25" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -2296,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:IX66"/>
+  <dimension ref="A5:IX70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:G25"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2320,30 +2365,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12">
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
     </row>
     <row r="7" spans="2:12" ht="30">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
     </row>
     <row r="8" spans="2:12" ht="30">
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2355,939 +2400,1981 @@
       <c r="E12"/>
     </row>
     <row r="13" spans="2:12" ht="111.95" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
     </row>
     <row r="14" spans="2:12" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
       <c r="K14"/>
       <c r="L14"/>
     </row>
     <row r="15" spans="2:12" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
     </row>
     <row r="16" spans="2:12" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="17" spans="1:258" ht="21.75" customHeight="1" thickTop="1">
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="75" t="s">
+      <c r="C17" s="80"/>
+      <c r="D17" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="75" t="s">
+      <c r="E17" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="76" t="s">
+      <c r="F17" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="76"/>
-    </row>
-    <row r="18" spans="1:258" s="70" customFormat="1" ht="57" customHeight="1">
-      <c r="A18" s="72"/>
-      <c r="B18" s="78" t="s">
+      <c r="G17" s="81"/>
+    </row>
+    <row r="18" spans="1:258" s="53" customFormat="1" ht="57" customHeight="1">
+      <c r="A18" s="55"/>
+      <c r="B18" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="79" t="s">
+      <c r="C18" s="71"/>
+      <c r="D18" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="81" t="s">
+      <c r="F18" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="81"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="71"/>
-      <c r="N18" s="71"/>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
-      <c r="Q18" s="71"/>
-      <c r="R18" s="71"/>
-      <c r="S18" s="71"/>
-      <c r="T18" s="71"/>
-      <c r="U18" s="71"/>
-      <c r="V18" s="71"/>
-      <c r="W18" s="71"/>
-      <c r="X18" s="71"/>
-      <c r="Y18" s="71"/>
-      <c r="Z18" s="71"/>
-      <c r="AA18" s="71"/>
-      <c r="AB18" s="71"/>
-      <c r="AC18" s="71"/>
-      <c r="AD18" s="71"/>
-      <c r="AE18" s="71"/>
-      <c r="AF18" s="71"/>
-      <c r="AG18" s="71"/>
-      <c r="AH18" s="71"/>
-      <c r="AI18" s="71"/>
-      <c r="AJ18" s="71"/>
-      <c r="AK18" s="71"/>
-      <c r="AL18" s="71"/>
-      <c r="AM18" s="71"/>
-      <c r="AN18" s="71"/>
-      <c r="AO18" s="71"/>
-      <c r="AP18" s="71"/>
-      <c r="AQ18" s="71"/>
-      <c r="AR18" s="71"/>
-      <c r="AS18" s="71"/>
-      <c r="AT18" s="71"/>
-      <c r="AU18" s="71"/>
-      <c r="AV18" s="71"/>
-      <c r="AW18" s="71"/>
-      <c r="AX18" s="71"/>
-      <c r="AY18" s="71"/>
-      <c r="AZ18" s="71"/>
-      <c r="BA18" s="71"/>
-      <c r="BB18" s="71"/>
-      <c r="BC18" s="71"/>
-      <c r="BD18" s="71"/>
-      <c r="BE18" s="71"/>
-      <c r="BF18" s="71"/>
-      <c r="BG18" s="71"/>
-      <c r="BH18" s="71"/>
-      <c r="BI18" s="71"/>
-      <c r="BJ18" s="71"/>
-      <c r="BK18" s="71"/>
-      <c r="BL18" s="71"/>
-      <c r="BM18" s="71"/>
-      <c r="BN18" s="71"/>
-      <c r="BO18" s="71"/>
-      <c r="BP18" s="71"/>
-      <c r="BQ18" s="71"/>
-      <c r="BR18" s="71"/>
-      <c r="BS18" s="71"/>
-      <c r="BT18" s="71"/>
-      <c r="BU18" s="71"/>
-      <c r="BV18" s="71"/>
-      <c r="BW18" s="71"/>
-      <c r="BX18" s="71"/>
-      <c r="BY18" s="71"/>
-      <c r="BZ18" s="71"/>
-      <c r="CA18" s="71"/>
-      <c r="CB18" s="71"/>
-      <c r="CC18" s="71"/>
-      <c r="CD18" s="71"/>
-      <c r="CE18" s="71"/>
-      <c r="CF18" s="71"/>
-      <c r="CG18" s="71"/>
-      <c r="CH18" s="71"/>
-      <c r="CI18" s="71"/>
-      <c r="CJ18" s="71"/>
-      <c r="CK18" s="71"/>
-      <c r="CL18" s="71"/>
-      <c r="CM18" s="71"/>
-      <c r="CN18" s="71"/>
-      <c r="CO18" s="71"/>
-      <c r="CP18" s="71"/>
-      <c r="CQ18" s="71"/>
-      <c r="CR18" s="71"/>
-      <c r="CS18" s="71"/>
-      <c r="CT18" s="71"/>
-      <c r="CU18" s="71"/>
-      <c r="CV18" s="71"/>
-      <c r="CW18" s="71"/>
-      <c r="CX18" s="71"/>
-      <c r="CY18" s="71"/>
-      <c r="CZ18" s="71"/>
-      <c r="DA18" s="71"/>
-      <c r="DB18" s="71"/>
-      <c r="DC18" s="71"/>
-      <c r="DD18" s="71"/>
-      <c r="DE18" s="71"/>
-      <c r="DF18" s="71"/>
-      <c r="DG18" s="71"/>
-      <c r="DH18" s="71"/>
-      <c r="DI18" s="71"/>
-      <c r="DJ18" s="71"/>
-      <c r="DK18" s="71"/>
-      <c r="DL18" s="71"/>
-      <c r="DM18" s="71"/>
-      <c r="DN18" s="71"/>
-      <c r="DO18" s="71"/>
-      <c r="DP18" s="71"/>
-      <c r="DQ18" s="71"/>
-      <c r="DR18" s="71"/>
-      <c r="DS18" s="71"/>
-      <c r="DT18" s="71"/>
-      <c r="DU18" s="71"/>
-      <c r="DV18" s="71"/>
-      <c r="DW18" s="71"/>
-      <c r="DX18" s="71"/>
-      <c r="DY18" s="71"/>
-      <c r="DZ18" s="71"/>
-      <c r="EA18" s="71"/>
-      <c r="EB18" s="71"/>
-      <c r="EC18" s="71"/>
-      <c r="ED18" s="71"/>
-      <c r="EE18" s="71"/>
-      <c r="EF18" s="71"/>
-      <c r="EG18" s="71"/>
-      <c r="EH18" s="71"/>
-      <c r="EI18" s="71"/>
-      <c r="EJ18" s="71"/>
-      <c r="EK18" s="71"/>
-      <c r="EL18" s="71"/>
-      <c r="EM18" s="71"/>
-      <c r="EN18" s="71"/>
-      <c r="EO18" s="71"/>
-      <c r="EP18" s="71"/>
-      <c r="EQ18" s="71"/>
-      <c r="ER18" s="71"/>
-      <c r="ES18" s="71"/>
-      <c r="ET18" s="71"/>
-      <c r="EU18" s="71"/>
-      <c r="EV18" s="71"/>
-      <c r="EW18" s="71"/>
-      <c r="EX18" s="71"/>
-      <c r="EY18" s="71"/>
-      <c r="EZ18" s="71"/>
-      <c r="FA18" s="71"/>
-      <c r="FB18" s="71"/>
-      <c r="FC18" s="71"/>
-      <c r="FD18" s="71"/>
-      <c r="FE18" s="71"/>
-      <c r="FF18" s="71"/>
-      <c r="FG18" s="71"/>
-      <c r="FH18" s="71"/>
-      <c r="FI18" s="71"/>
-      <c r="FJ18" s="71"/>
-      <c r="FK18" s="71"/>
-      <c r="FL18" s="71"/>
-      <c r="FM18" s="71"/>
-      <c r="FN18" s="71"/>
-      <c r="FO18" s="71"/>
-      <c r="FP18" s="71"/>
-      <c r="FQ18" s="71"/>
-      <c r="FR18" s="71"/>
-      <c r="FS18" s="71"/>
-      <c r="FT18" s="71"/>
-      <c r="FU18" s="71"/>
-      <c r="FV18" s="71"/>
-      <c r="FW18" s="71"/>
-      <c r="FX18" s="71"/>
-      <c r="FY18" s="71"/>
-      <c r="FZ18" s="71"/>
-      <c r="GA18" s="71"/>
-      <c r="GB18" s="71"/>
-      <c r="GC18" s="71"/>
-      <c r="GD18" s="71"/>
-      <c r="GE18" s="71"/>
-      <c r="GF18" s="71"/>
-      <c r="GG18" s="71"/>
-      <c r="GH18" s="71"/>
-      <c r="GI18" s="71"/>
-      <c r="GJ18" s="71"/>
-      <c r="GK18" s="71"/>
-      <c r="GL18" s="71"/>
-      <c r="GM18" s="71"/>
-      <c r="GN18" s="71"/>
-      <c r="GO18" s="71"/>
-      <c r="GP18" s="71"/>
-      <c r="GQ18" s="71"/>
-      <c r="GR18" s="71"/>
-      <c r="GS18" s="71"/>
-      <c r="GT18" s="71"/>
-      <c r="GU18" s="71"/>
-      <c r="GV18" s="71"/>
-      <c r="GW18" s="71"/>
-      <c r="GX18" s="71"/>
-      <c r="GY18" s="71"/>
-      <c r="GZ18" s="71"/>
-      <c r="HA18" s="71"/>
-      <c r="HB18" s="71"/>
-      <c r="HC18" s="71"/>
-      <c r="HD18" s="71"/>
-      <c r="HE18" s="71"/>
-      <c r="HF18" s="71"/>
-      <c r="HG18" s="71"/>
-      <c r="HH18" s="71"/>
-      <c r="HI18" s="71"/>
-      <c r="HJ18" s="71"/>
-      <c r="HK18" s="71"/>
-      <c r="HL18" s="71"/>
-      <c r="HM18" s="71"/>
-      <c r="HN18" s="71"/>
-      <c r="HO18" s="71"/>
-      <c r="HP18" s="71"/>
-      <c r="HQ18" s="71"/>
-      <c r="HR18" s="71"/>
-      <c r="HS18" s="71"/>
-      <c r="HT18" s="71"/>
-      <c r="HU18" s="71"/>
-      <c r="HV18" s="71"/>
-      <c r="HW18" s="71"/>
-      <c r="HX18" s="71"/>
-      <c r="HY18" s="71"/>
-      <c r="HZ18" s="71"/>
-      <c r="IA18" s="71"/>
-      <c r="IB18" s="71"/>
-      <c r="IC18" s="71"/>
-      <c r="ID18" s="71"/>
-      <c r="IE18" s="71"/>
-      <c r="IF18" s="71"/>
-      <c r="IG18" s="71"/>
-      <c r="IH18" s="71"/>
-      <c r="II18" s="71"/>
-      <c r="IJ18" s="71"/>
-      <c r="IK18" s="71"/>
-      <c r="IL18" s="71"/>
-      <c r="IM18" s="71"/>
-      <c r="IN18" s="71"/>
-      <c r="IO18" s="71"/>
-      <c r="IP18" s="71"/>
-      <c r="IQ18" s="71"/>
-      <c r="IR18" s="71"/>
-      <c r="IS18" s="71"/>
-      <c r="IT18" s="71"/>
-      <c r="IU18" s="71"/>
-      <c r="IV18" s="71"/>
-      <c r="IW18" s="71"/>
-      <c r="IX18" s="71"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="54"/>
+      <c r="AA18" s="54"/>
+      <c r="AB18" s="54"/>
+      <c r="AC18" s="54"/>
+      <c r="AD18" s="54"/>
+      <c r="AE18" s="54"/>
+      <c r="AF18" s="54"/>
+      <c r="AG18" s="54"/>
+      <c r="AH18" s="54"/>
+      <c r="AI18" s="54"/>
+      <c r="AJ18" s="54"/>
+      <c r="AK18" s="54"/>
+      <c r="AL18" s="54"/>
+      <c r="AM18" s="54"/>
+      <c r="AN18" s="54"/>
+      <c r="AO18" s="54"/>
+      <c r="AP18" s="54"/>
+      <c r="AQ18" s="54"/>
+      <c r="AR18" s="54"/>
+      <c r="AS18" s="54"/>
+      <c r="AT18" s="54"/>
+      <c r="AU18" s="54"/>
+      <c r="AV18" s="54"/>
+      <c r="AW18" s="54"/>
+      <c r="AX18" s="54"/>
+      <c r="AY18" s="54"/>
+      <c r="AZ18" s="54"/>
+      <c r="BA18" s="54"/>
+      <c r="BB18" s="54"/>
+      <c r="BC18" s="54"/>
+      <c r="BD18" s="54"/>
+      <c r="BE18" s="54"/>
+      <c r="BF18" s="54"/>
+      <c r="BG18" s="54"/>
+      <c r="BH18" s="54"/>
+      <c r="BI18" s="54"/>
+      <c r="BJ18" s="54"/>
+      <c r="BK18" s="54"/>
+      <c r="BL18" s="54"/>
+      <c r="BM18" s="54"/>
+      <c r="BN18" s="54"/>
+      <c r="BO18" s="54"/>
+      <c r="BP18" s="54"/>
+      <c r="BQ18" s="54"/>
+      <c r="BR18" s="54"/>
+      <c r="BS18" s="54"/>
+      <c r="BT18" s="54"/>
+      <c r="BU18" s="54"/>
+      <c r="BV18" s="54"/>
+      <c r="BW18" s="54"/>
+      <c r="BX18" s="54"/>
+      <c r="BY18" s="54"/>
+      <c r="BZ18" s="54"/>
+      <c r="CA18" s="54"/>
+      <c r="CB18" s="54"/>
+      <c r="CC18" s="54"/>
+      <c r="CD18" s="54"/>
+      <c r="CE18" s="54"/>
+      <c r="CF18" s="54"/>
+      <c r="CG18" s="54"/>
+      <c r="CH18" s="54"/>
+      <c r="CI18" s="54"/>
+      <c r="CJ18" s="54"/>
+      <c r="CK18" s="54"/>
+      <c r="CL18" s="54"/>
+      <c r="CM18" s="54"/>
+      <c r="CN18" s="54"/>
+      <c r="CO18" s="54"/>
+      <c r="CP18" s="54"/>
+      <c r="CQ18" s="54"/>
+      <c r="CR18" s="54"/>
+      <c r="CS18" s="54"/>
+      <c r="CT18" s="54"/>
+      <c r="CU18" s="54"/>
+      <c r="CV18" s="54"/>
+      <c r="CW18" s="54"/>
+      <c r="CX18" s="54"/>
+      <c r="CY18" s="54"/>
+      <c r="CZ18" s="54"/>
+      <c r="DA18" s="54"/>
+      <c r="DB18" s="54"/>
+      <c r="DC18" s="54"/>
+      <c r="DD18" s="54"/>
+      <c r="DE18" s="54"/>
+      <c r="DF18" s="54"/>
+      <c r="DG18" s="54"/>
+      <c r="DH18" s="54"/>
+      <c r="DI18" s="54"/>
+      <c r="DJ18" s="54"/>
+      <c r="DK18" s="54"/>
+      <c r="DL18" s="54"/>
+      <c r="DM18" s="54"/>
+      <c r="DN18" s="54"/>
+      <c r="DO18" s="54"/>
+      <c r="DP18" s="54"/>
+      <c r="DQ18" s="54"/>
+      <c r="DR18" s="54"/>
+      <c r="DS18" s="54"/>
+      <c r="DT18" s="54"/>
+      <c r="DU18" s="54"/>
+      <c r="DV18" s="54"/>
+      <c r="DW18" s="54"/>
+      <c r="DX18" s="54"/>
+      <c r="DY18" s="54"/>
+      <c r="DZ18" s="54"/>
+      <c r="EA18" s="54"/>
+      <c r="EB18" s="54"/>
+      <c r="EC18" s="54"/>
+      <c r="ED18" s="54"/>
+      <c r="EE18" s="54"/>
+      <c r="EF18" s="54"/>
+      <c r="EG18" s="54"/>
+      <c r="EH18" s="54"/>
+      <c r="EI18" s="54"/>
+      <c r="EJ18" s="54"/>
+      <c r="EK18" s="54"/>
+      <c r="EL18" s="54"/>
+      <c r="EM18" s="54"/>
+      <c r="EN18" s="54"/>
+      <c r="EO18" s="54"/>
+      <c r="EP18" s="54"/>
+      <c r="EQ18" s="54"/>
+      <c r="ER18" s="54"/>
+      <c r="ES18" s="54"/>
+      <c r="ET18" s="54"/>
+      <c r="EU18" s="54"/>
+      <c r="EV18" s="54"/>
+      <c r="EW18" s="54"/>
+      <c r="EX18" s="54"/>
+      <c r="EY18" s="54"/>
+      <c r="EZ18" s="54"/>
+      <c r="FA18" s="54"/>
+      <c r="FB18" s="54"/>
+      <c r="FC18" s="54"/>
+      <c r="FD18" s="54"/>
+      <c r="FE18" s="54"/>
+      <c r="FF18" s="54"/>
+      <c r="FG18" s="54"/>
+      <c r="FH18" s="54"/>
+      <c r="FI18" s="54"/>
+      <c r="FJ18" s="54"/>
+      <c r="FK18" s="54"/>
+      <c r="FL18" s="54"/>
+      <c r="FM18" s="54"/>
+      <c r="FN18" s="54"/>
+      <c r="FO18" s="54"/>
+      <c r="FP18" s="54"/>
+      <c r="FQ18" s="54"/>
+      <c r="FR18" s="54"/>
+      <c r="FS18" s="54"/>
+      <c r="FT18" s="54"/>
+      <c r="FU18" s="54"/>
+      <c r="FV18" s="54"/>
+      <c r="FW18" s="54"/>
+      <c r="FX18" s="54"/>
+      <c r="FY18" s="54"/>
+      <c r="FZ18" s="54"/>
+      <c r="GA18" s="54"/>
+      <c r="GB18" s="54"/>
+      <c r="GC18" s="54"/>
+      <c r="GD18" s="54"/>
+      <c r="GE18" s="54"/>
+      <c r="GF18" s="54"/>
+      <c r="GG18" s="54"/>
+      <c r="GH18" s="54"/>
+      <c r="GI18" s="54"/>
+      <c r="GJ18" s="54"/>
+      <c r="GK18" s="54"/>
+      <c r="GL18" s="54"/>
+      <c r="GM18" s="54"/>
+      <c r="GN18" s="54"/>
+      <c r="GO18" s="54"/>
+      <c r="GP18" s="54"/>
+      <c r="GQ18" s="54"/>
+      <c r="GR18" s="54"/>
+      <c r="GS18" s="54"/>
+      <c r="GT18" s="54"/>
+      <c r="GU18" s="54"/>
+      <c r="GV18" s="54"/>
+      <c r="GW18" s="54"/>
+      <c r="GX18" s="54"/>
+      <c r="GY18" s="54"/>
+      <c r="GZ18" s="54"/>
+      <c r="HA18" s="54"/>
+      <c r="HB18" s="54"/>
+      <c r="HC18" s="54"/>
+      <c r="HD18" s="54"/>
+      <c r="HE18" s="54"/>
+      <c r="HF18" s="54"/>
+      <c r="HG18" s="54"/>
+      <c r="HH18" s="54"/>
+      <c r="HI18" s="54"/>
+      <c r="HJ18" s="54"/>
+      <c r="HK18" s="54"/>
+      <c r="HL18" s="54"/>
+      <c r="HM18" s="54"/>
+      <c r="HN18" s="54"/>
+      <c r="HO18" s="54"/>
+      <c r="HP18" s="54"/>
+      <c r="HQ18" s="54"/>
+      <c r="HR18" s="54"/>
+      <c r="HS18" s="54"/>
+      <c r="HT18" s="54"/>
+      <c r="HU18" s="54"/>
+      <c r="HV18" s="54"/>
+      <c r="HW18" s="54"/>
+      <c r="HX18" s="54"/>
+      <c r="HY18" s="54"/>
+      <c r="HZ18" s="54"/>
+      <c r="IA18" s="54"/>
+      <c r="IB18" s="54"/>
+      <c r="IC18" s="54"/>
+      <c r="ID18" s="54"/>
+      <c r="IE18" s="54"/>
+      <c r="IF18" s="54"/>
+      <c r="IG18" s="54"/>
+      <c r="IH18" s="54"/>
+      <c r="II18" s="54"/>
+      <c r="IJ18" s="54"/>
+      <c r="IK18" s="54"/>
+      <c r="IL18" s="54"/>
+      <c r="IM18" s="54"/>
+      <c r="IN18" s="54"/>
+      <c r="IO18" s="54"/>
+      <c r="IP18" s="54"/>
+      <c r="IQ18" s="54"/>
+      <c r="IR18" s="54"/>
+      <c r="IS18" s="54"/>
+      <c r="IT18" s="54"/>
+      <c r="IU18" s="54"/>
+      <c r="IV18" s="54"/>
+      <c r="IW18" s="54"/>
+      <c r="IX18" s="54"/>
     </row>
     <row r="19" spans="1:258" ht="47.25" customHeight="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="79" t="s">
+      <c r="C19" s="73"/>
+      <c r="D19" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="88" t="s">
+      <c r="E19" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="85" t="s">
+      <c r="F19" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="86"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="36"/>
     </row>
     <row r="20" spans="1:258" ht="47.25" customHeight="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="84"/>
-      <c r="D20" s="79" t="s">
+      <c r="C20" s="76"/>
+      <c r="D20" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="80" t="s">
+      <c r="E20" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="85" t="s">
+      <c r="F20" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="86"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:258" ht="47.25" customHeight="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="84"/>
-      <c r="D21" s="79" t="s">
+      <c r="C21" s="76"/>
+      <c r="D21" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="87" t="s">
+      <c r="E21" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="85" t="s">
+      <c r="F21" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="86"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="36"/>
     </row>
     <row r="22" spans="1:258" ht="66" customHeight="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="84"/>
-      <c r="D22" s="79" t="s">
+      <c r="C22" s="76"/>
+      <c r="D22" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="79" t="s">
+      <c r="E22" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="85" t="s">
+      <c r="F22" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="86"/>
+      <c r="G22" s="70"/>
       <c r="H22" s="36"/>
     </row>
     <row r="23" spans="1:258" ht="66" customHeight="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="90"/>
-      <c r="D23" s="79" t="s">
+      <c r="C23" s="68"/>
+      <c r="D23" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="79" t="s">
+      <c r="E23" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="85" t="s">
+      <c r="F23" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="86"/>
+      <c r="G23" s="70"/>
       <c r="H23" s="36"/>
     </row>
     <row r="24" spans="1:258" ht="66" customHeight="1">
       <c r="A24" s="30"/>
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="90"/>
-      <c r="D24" s="79" t="s">
+      <c r="C24" s="68"/>
+      <c r="D24" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="79" t="s">
+      <c r="E24" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="85" t="s">
+      <c r="F24" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="86"/>
+      <c r="G24" s="70"/>
       <c r="H24" s="36"/>
     </row>
-    <row r="25" spans="1:258" s="94" customFormat="1" ht="84.75" customHeight="1">
-      <c r="A25" s="91"/>
-      <c r="B25" s="89" t="s">
+    <row r="25" spans="1:258" s="66" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A25" s="63"/>
+      <c r="B25" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="90"/>
-      <c r="D25" s="79" t="s">
+      <c r="C25" s="68"/>
+      <c r="D25" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="79" t="s">
+      <c r="E25" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="85" t="s">
+      <c r="F25" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="86"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
-      <c r="K25" s="93"/>
-      <c r="L25" s="93"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="93"/>
-      <c r="O25" s="93"/>
-      <c r="P25" s="93"/>
-      <c r="Q25" s="93"/>
-      <c r="R25" s="93"/>
-      <c r="S25" s="93"/>
-      <c r="T25" s="93"/>
-      <c r="U25" s="93"/>
-      <c r="V25" s="93"/>
-      <c r="W25" s="93"/>
-      <c r="X25" s="93"/>
-      <c r="Y25" s="93"/>
-      <c r="Z25" s="93"/>
-      <c r="AA25" s="93"/>
-      <c r="AB25" s="93"/>
-      <c r="AC25" s="93"/>
-      <c r="AD25" s="93"/>
-      <c r="AE25" s="93"/>
-      <c r="AF25" s="93"/>
-      <c r="AG25" s="93"/>
-      <c r="AH25" s="93"/>
-      <c r="AI25" s="93"/>
-      <c r="AJ25" s="93"/>
-      <c r="AK25" s="93"/>
-      <c r="AL25" s="93"/>
-      <c r="AM25" s="93"/>
-      <c r="AN25" s="93"/>
-      <c r="AO25" s="93"/>
-      <c r="AP25" s="93"/>
-      <c r="AQ25" s="93"/>
-      <c r="AR25" s="93"/>
-      <c r="AS25" s="93"/>
-      <c r="AT25" s="93"/>
-      <c r="AU25" s="93"/>
-      <c r="AV25" s="93"/>
-      <c r="AW25" s="93"/>
-      <c r="AX25" s="93"/>
-      <c r="AY25" s="93"/>
-      <c r="AZ25" s="93"/>
-      <c r="BA25" s="93"/>
-      <c r="BB25" s="93"/>
-      <c r="BC25" s="93"/>
-      <c r="BD25" s="93"/>
-      <c r="BE25" s="93"/>
-      <c r="BF25" s="93"/>
-      <c r="BG25" s="93"/>
-      <c r="BH25" s="93"/>
-      <c r="BI25" s="93"/>
-      <c r="BJ25" s="93"/>
-      <c r="BK25" s="93"/>
-      <c r="BL25" s="93"/>
-      <c r="BM25" s="93"/>
-      <c r="BN25" s="93"/>
-      <c r="BO25" s="93"/>
-      <c r="BP25" s="93"/>
-      <c r="BQ25" s="93"/>
-      <c r="BR25" s="93"/>
-      <c r="BS25" s="93"/>
-      <c r="BT25" s="93"/>
-      <c r="BU25" s="93"/>
-      <c r="BV25" s="93"/>
-      <c r="BW25" s="93"/>
-      <c r="BX25" s="93"/>
-      <c r="BY25" s="93"/>
-      <c r="BZ25" s="93"/>
-      <c r="CA25" s="93"/>
-      <c r="CB25" s="93"/>
-      <c r="CC25" s="93"/>
-      <c r="CD25" s="93"/>
-      <c r="CE25" s="93"/>
-      <c r="CF25" s="93"/>
-      <c r="CG25" s="93"/>
-      <c r="CH25" s="93"/>
-      <c r="CI25" s="93"/>
-      <c r="CJ25" s="93"/>
-      <c r="CK25" s="93"/>
-      <c r="CL25" s="93"/>
-      <c r="CM25" s="93"/>
-      <c r="CN25" s="93"/>
-      <c r="CO25" s="93"/>
-      <c r="CP25" s="93"/>
-      <c r="CQ25" s="93"/>
-      <c r="CR25" s="93"/>
-      <c r="CS25" s="93"/>
-      <c r="CT25" s="93"/>
-      <c r="CU25" s="93"/>
-      <c r="CV25" s="93"/>
-      <c r="CW25" s="93"/>
-      <c r="CX25" s="93"/>
-      <c r="CY25" s="93"/>
-      <c r="CZ25" s="93"/>
-      <c r="DA25" s="93"/>
-      <c r="DB25" s="93"/>
-      <c r="DC25" s="93"/>
-      <c r="DD25" s="93"/>
-      <c r="DE25" s="93"/>
-      <c r="DF25" s="93"/>
-      <c r="DG25" s="93"/>
-      <c r="DH25" s="93"/>
-      <c r="DI25" s="93"/>
-      <c r="DJ25" s="93"/>
-      <c r="DK25" s="93"/>
-      <c r="DL25" s="93"/>
-      <c r="DM25" s="93"/>
-      <c r="DN25" s="93"/>
-      <c r="DO25" s="93"/>
-      <c r="DP25" s="93"/>
-      <c r="DQ25" s="93"/>
-      <c r="DR25" s="93"/>
-      <c r="DS25" s="93"/>
-      <c r="DT25" s="93"/>
-      <c r="DU25" s="93"/>
-      <c r="DV25" s="93"/>
-      <c r="DW25" s="93"/>
-      <c r="DX25" s="93"/>
-      <c r="DY25" s="93"/>
-      <c r="DZ25" s="93"/>
-      <c r="EA25" s="93"/>
-      <c r="EB25" s="93"/>
-      <c r="EC25" s="93"/>
-      <c r="ED25" s="93"/>
-      <c r="EE25" s="93"/>
-      <c r="EF25" s="93"/>
-      <c r="EG25" s="93"/>
-      <c r="EH25" s="93"/>
-      <c r="EI25" s="93"/>
-      <c r="EJ25" s="93"/>
-      <c r="EK25" s="93"/>
-      <c r="EL25" s="93"/>
-      <c r="EM25" s="93"/>
-      <c r="EN25" s="93"/>
-      <c r="EO25" s="93"/>
-      <c r="EP25" s="93"/>
-      <c r="EQ25" s="93"/>
-      <c r="ER25" s="93"/>
-      <c r="ES25" s="93"/>
-      <c r="ET25" s="93"/>
-      <c r="EU25" s="93"/>
-      <c r="EV25" s="93"/>
-      <c r="EW25" s="93"/>
-      <c r="EX25" s="93"/>
-      <c r="EY25" s="93"/>
-      <c r="EZ25" s="93"/>
-      <c r="FA25" s="93"/>
-      <c r="FB25" s="93"/>
-      <c r="FC25" s="93"/>
-      <c r="FD25" s="93"/>
-      <c r="FE25" s="93"/>
-      <c r="FF25" s="93"/>
-      <c r="FG25" s="93"/>
-      <c r="FH25" s="93"/>
-      <c r="FI25" s="93"/>
-      <c r="FJ25" s="93"/>
-      <c r="FK25" s="93"/>
-      <c r="FL25" s="93"/>
-      <c r="FM25" s="93"/>
-      <c r="FN25" s="93"/>
-      <c r="FO25" s="93"/>
-      <c r="FP25" s="93"/>
-      <c r="FQ25" s="93"/>
-      <c r="FR25" s="93"/>
-      <c r="FS25" s="93"/>
-      <c r="FT25" s="93"/>
-      <c r="FU25" s="93"/>
-      <c r="FV25" s="93"/>
-      <c r="FW25" s="93"/>
-      <c r="FX25" s="93"/>
-      <c r="FY25" s="93"/>
-      <c r="FZ25" s="93"/>
-      <c r="GA25" s="93"/>
-      <c r="GB25" s="93"/>
-      <c r="GC25" s="93"/>
-      <c r="GD25" s="93"/>
-      <c r="GE25" s="93"/>
-      <c r="GF25" s="93"/>
-      <c r="GG25" s="93"/>
-      <c r="GH25" s="93"/>
-      <c r="GI25" s="93"/>
-      <c r="GJ25" s="93"/>
-      <c r="GK25" s="93"/>
-      <c r="GL25" s="93"/>
-      <c r="GM25" s="93"/>
-      <c r="GN25" s="93"/>
-      <c r="GO25" s="93"/>
-      <c r="GP25" s="93"/>
-      <c r="GQ25" s="93"/>
-      <c r="GR25" s="93"/>
-      <c r="GS25" s="93"/>
-      <c r="GT25" s="93"/>
-      <c r="GU25" s="93"/>
-      <c r="GV25" s="93"/>
-      <c r="GW25" s="93"/>
-      <c r="GX25" s="93"/>
-      <c r="GY25" s="93"/>
-      <c r="GZ25" s="93"/>
-      <c r="HA25" s="93"/>
-      <c r="HB25" s="93"/>
-      <c r="HC25" s="93"/>
-      <c r="HD25" s="93"/>
-      <c r="HE25" s="93"/>
-      <c r="HF25" s="93"/>
-      <c r="HG25" s="93"/>
-      <c r="HH25" s="93"/>
-      <c r="HI25" s="93"/>
-      <c r="HJ25" s="93"/>
-      <c r="HK25" s="93"/>
-      <c r="HL25" s="93"/>
-      <c r="HM25" s="93"/>
-      <c r="HN25" s="93"/>
-      <c r="HO25" s="93"/>
-      <c r="HP25" s="93"/>
-      <c r="HQ25" s="93"/>
-      <c r="HR25" s="93"/>
-      <c r="HS25" s="93"/>
-      <c r="HT25" s="93"/>
-      <c r="HU25" s="93"/>
-      <c r="HV25" s="93"/>
-      <c r="HW25" s="93"/>
-      <c r="HX25" s="93"/>
-      <c r="HY25" s="93"/>
-      <c r="HZ25" s="93"/>
-      <c r="IA25" s="93"/>
-      <c r="IB25" s="93"/>
-      <c r="IC25" s="93"/>
-      <c r="ID25" s="93"/>
-      <c r="IE25" s="93"/>
-      <c r="IF25" s="93"/>
-      <c r="IG25" s="93"/>
-      <c r="IH25" s="93"/>
-      <c r="II25" s="93"/>
-      <c r="IJ25" s="93"/>
-      <c r="IK25" s="93"/>
-      <c r="IL25" s="93"/>
-      <c r="IM25" s="93"/>
-      <c r="IN25" s="93"/>
-      <c r="IO25" s="93"/>
-      <c r="IP25" s="93"/>
-      <c r="IQ25" s="93"/>
-      <c r="IR25" s="93"/>
-      <c r="IS25" s="93"/>
-      <c r="IT25" s="93"/>
-      <c r="IU25" s="93"/>
-      <c r="IV25" s="93"/>
-      <c r="IW25" s="93"/>
-      <c r="IX25" s="93"/>
-    </row>
-    <row r="26" spans="1:258" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="B26" s="52"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="53"/>
-    </row>
-    <row r="27" spans="1:258" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B27" s="69" t="s">
+      <c r="G25" s="70"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="65"/>
+      <c r="U25" s="65"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="65"/>
+      <c r="X25" s="65"/>
+      <c r="Y25" s="65"/>
+      <c r="Z25" s="65"/>
+      <c r="AA25" s="65"/>
+      <c r="AB25" s="65"/>
+      <c r="AC25" s="65"/>
+      <c r="AD25" s="65"/>
+      <c r="AE25" s="65"/>
+      <c r="AF25" s="65"/>
+      <c r="AG25" s="65"/>
+      <c r="AH25" s="65"/>
+      <c r="AI25" s="65"/>
+      <c r="AJ25" s="65"/>
+      <c r="AK25" s="65"/>
+      <c r="AL25" s="65"/>
+      <c r="AM25" s="65"/>
+      <c r="AN25" s="65"/>
+      <c r="AO25" s="65"/>
+      <c r="AP25" s="65"/>
+      <c r="AQ25" s="65"/>
+      <c r="AR25" s="65"/>
+      <c r="AS25" s="65"/>
+      <c r="AT25" s="65"/>
+      <c r="AU25" s="65"/>
+      <c r="AV25" s="65"/>
+      <c r="AW25" s="65"/>
+      <c r="AX25" s="65"/>
+      <c r="AY25" s="65"/>
+      <c r="AZ25" s="65"/>
+      <c r="BA25" s="65"/>
+      <c r="BB25" s="65"/>
+      <c r="BC25" s="65"/>
+      <c r="BD25" s="65"/>
+      <c r="BE25" s="65"/>
+      <c r="BF25" s="65"/>
+      <c r="BG25" s="65"/>
+      <c r="BH25" s="65"/>
+      <c r="BI25" s="65"/>
+      <c r="BJ25" s="65"/>
+      <c r="BK25" s="65"/>
+      <c r="BL25" s="65"/>
+      <c r="BM25" s="65"/>
+      <c r="BN25" s="65"/>
+      <c r="BO25" s="65"/>
+      <c r="BP25" s="65"/>
+      <c r="BQ25" s="65"/>
+      <c r="BR25" s="65"/>
+      <c r="BS25" s="65"/>
+      <c r="BT25" s="65"/>
+      <c r="BU25" s="65"/>
+      <c r="BV25" s="65"/>
+      <c r="BW25" s="65"/>
+      <c r="BX25" s="65"/>
+      <c r="BY25" s="65"/>
+      <c r="BZ25" s="65"/>
+      <c r="CA25" s="65"/>
+      <c r="CB25" s="65"/>
+      <c r="CC25" s="65"/>
+      <c r="CD25" s="65"/>
+      <c r="CE25" s="65"/>
+      <c r="CF25" s="65"/>
+      <c r="CG25" s="65"/>
+      <c r="CH25" s="65"/>
+      <c r="CI25" s="65"/>
+      <c r="CJ25" s="65"/>
+      <c r="CK25" s="65"/>
+      <c r="CL25" s="65"/>
+      <c r="CM25" s="65"/>
+      <c r="CN25" s="65"/>
+      <c r="CO25" s="65"/>
+      <c r="CP25" s="65"/>
+      <c r="CQ25" s="65"/>
+      <c r="CR25" s="65"/>
+      <c r="CS25" s="65"/>
+      <c r="CT25" s="65"/>
+      <c r="CU25" s="65"/>
+      <c r="CV25" s="65"/>
+      <c r="CW25" s="65"/>
+      <c r="CX25" s="65"/>
+      <c r="CY25" s="65"/>
+      <c r="CZ25" s="65"/>
+      <c r="DA25" s="65"/>
+      <c r="DB25" s="65"/>
+      <c r="DC25" s="65"/>
+      <c r="DD25" s="65"/>
+      <c r="DE25" s="65"/>
+      <c r="DF25" s="65"/>
+      <c r="DG25" s="65"/>
+      <c r="DH25" s="65"/>
+      <c r="DI25" s="65"/>
+      <c r="DJ25" s="65"/>
+      <c r="DK25" s="65"/>
+      <c r="DL25" s="65"/>
+      <c r="DM25" s="65"/>
+      <c r="DN25" s="65"/>
+      <c r="DO25" s="65"/>
+      <c r="DP25" s="65"/>
+      <c r="DQ25" s="65"/>
+      <c r="DR25" s="65"/>
+      <c r="DS25" s="65"/>
+      <c r="DT25" s="65"/>
+      <c r="DU25" s="65"/>
+      <c r="DV25" s="65"/>
+      <c r="DW25" s="65"/>
+      <c r="DX25" s="65"/>
+      <c r="DY25" s="65"/>
+      <c r="DZ25" s="65"/>
+      <c r="EA25" s="65"/>
+      <c r="EB25" s="65"/>
+      <c r="EC25" s="65"/>
+      <c r="ED25" s="65"/>
+      <c r="EE25" s="65"/>
+      <c r="EF25" s="65"/>
+      <c r="EG25" s="65"/>
+      <c r="EH25" s="65"/>
+      <c r="EI25" s="65"/>
+      <c r="EJ25" s="65"/>
+      <c r="EK25" s="65"/>
+      <c r="EL25" s="65"/>
+      <c r="EM25" s="65"/>
+      <c r="EN25" s="65"/>
+      <c r="EO25" s="65"/>
+      <c r="EP25" s="65"/>
+      <c r="EQ25" s="65"/>
+      <c r="ER25" s="65"/>
+      <c r="ES25" s="65"/>
+      <c r="ET25" s="65"/>
+      <c r="EU25" s="65"/>
+      <c r="EV25" s="65"/>
+      <c r="EW25" s="65"/>
+      <c r="EX25" s="65"/>
+      <c r="EY25" s="65"/>
+      <c r="EZ25" s="65"/>
+      <c r="FA25" s="65"/>
+      <c r="FB25" s="65"/>
+      <c r="FC25" s="65"/>
+      <c r="FD25" s="65"/>
+      <c r="FE25" s="65"/>
+      <c r="FF25" s="65"/>
+      <c r="FG25" s="65"/>
+      <c r="FH25" s="65"/>
+      <c r="FI25" s="65"/>
+      <c r="FJ25" s="65"/>
+      <c r="FK25" s="65"/>
+      <c r="FL25" s="65"/>
+      <c r="FM25" s="65"/>
+      <c r="FN25" s="65"/>
+      <c r="FO25" s="65"/>
+      <c r="FP25" s="65"/>
+      <c r="FQ25" s="65"/>
+      <c r="FR25" s="65"/>
+      <c r="FS25" s="65"/>
+      <c r="FT25" s="65"/>
+      <c r="FU25" s="65"/>
+      <c r="FV25" s="65"/>
+      <c r="FW25" s="65"/>
+      <c r="FX25" s="65"/>
+      <c r="FY25" s="65"/>
+      <c r="FZ25" s="65"/>
+      <c r="GA25" s="65"/>
+      <c r="GB25" s="65"/>
+      <c r="GC25" s="65"/>
+      <c r="GD25" s="65"/>
+      <c r="GE25" s="65"/>
+      <c r="GF25" s="65"/>
+      <c r="GG25" s="65"/>
+      <c r="GH25" s="65"/>
+      <c r="GI25" s="65"/>
+      <c r="GJ25" s="65"/>
+      <c r="GK25" s="65"/>
+      <c r="GL25" s="65"/>
+      <c r="GM25" s="65"/>
+      <c r="GN25" s="65"/>
+      <c r="GO25" s="65"/>
+      <c r="GP25" s="65"/>
+      <c r="GQ25" s="65"/>
+      <c r="GR25" s="65"/>
+      <c r="GS25" s="65"/>
+      <c r="GT25" s="65"/>
+      <c r="GU25" s="65"/>
+      <c r="GV25" s="65"/>
+      <c r="GW25" s="65"/>
+      <c r="GX25" s="65"/>
+      <c r="GY25" s="65"/>
+      <c r="GZ25" s="65"/>
+      <c r="HA25" s="65"/>
+      <c r="HB25" s="65"/>
+      <c r="HC25" s="65"/>
+      <c r="HD25" s="65"/>
+      <c r="HE25" s="65"/>
+      <c r="HF25" s="65"/>
+      <c r="HG25" s="65"/>
+      <c r="HH25" s="65"/>
+      <c r="HI25" s="65"/>
+      <c r="HJ25" s="65"/>
+      <c r="HK25" s="65"/>
+      <c r="HL25" s="65"/>
+      <c r="HM25" s="65"/>
+      <c r="HN25" s="65"/>
+      <c r="HO25" s="65"/>
+      <c r="HP25" s="65"/>
+      <c r="HQ25" s="65"/>
+      <c r="HR25" s="65"/>
+      <c r="HS25" s="65"/>
+      <c r="HT25" s="65"/>
+      <c r="HU25" s="65"/>
+      <c r="HV25" s="65"/>
+      <c r="HW25" s="65"/>
+      <c r="HX25" s="65"/>
+      <c r="HY25" s="65"/>
+      <c r="HZ25" s="65"/>
+      <c r="IA25" s="65"/>
+      <c r="IB25" s="65"/>
+      <c r="IC25" s="65"/>
+      <c r="ID25" s="65"/>
+      <c r="IE25" s="65"/>
+      <c r="IF25" s="65"/>
+      <c r="IG25" s="65"/>
+      <c r="IH25" s="65"/>
+      <c r="II25" s="65"/>
+      <c r="IJ25" s="65"/>
+      <c r="IK25" s="65"/>
+      <c r="IL25" s="65"/>
+      <c r="IM25" s="65"/>
+      <c r="IN25" s="65"/>
+      <c r="IO25" s="65"/>
+      <c r="IP25" s="65"/>
+      <c r="IQ25" s="65"/>
+      <c r="IR25" s="65"/>
+      <c r="IS25" s="65"/>
+      <c r="IT25" s="65"/>
+      <c r="IU25" s="65"/>
+      <c r="IV25" s="65"/>
+      <c r="IW25" s="65"/>
+      <c r="IX25" s="65"/>
+    </row>
+    <row r="26" spans="1:258" s="66" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A26" s="63"/>
+      <c r="B26" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="71"/>
+      <c r="D26" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="70"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65"/>
+      <c r="T26" s="65"/>
+      <c r="U26" s="65"/>
+      <c r="V26" s="65"/>
+      <c r="W26" s="65"/>
+      <c r="X26" s="65"/>
+      <c r="Y26" s="65"/>
+      <c r="Z26" s="65"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
+      <c r="AC26" s="65"/>
+      <c r="AD26" s="65"/>
+      <c r="AE26" s="65"/>
+      <c r="AF26" s="65"/>
+      <c r="AG26" s="65"/>
+      <c r="AH26" s="65"/>
+      <c r="AI26" s="65"/>
+      <c r="AJ26" s="65"/>
+      <c r="AK26" s="65"/>
+      <c r="AL26" s="65"/>
+      <c r="AM26" s="65"/>
+      <c r="AN26" s="65"/>
+      <c r="AO26" s="65"/>
+      <c r="AP26" s="65"/>
+      <c r="AQ26" s="65"/>
+      <c r="AR26" s="65"/>
+      <c r="AS26" s="65"/>
+      <c r="AT26" s="65"/>
+      <c r="AU26" s="65"/>
+      <c r="AV26" s="65"/>
+      <c r="AW26" s="65"/>
+      <c r="AX26" s="65"/>
+      <c r="AY26" s="65"/>
+      <c r="AZ26" s="65"/>
+      <c r="BA26" s="65"/>
+      <c r="BB26" s="65"/>
+      <c r="BC26" s="65"/>
+      <c r="BD26" s="65"/>
+      <c r="BE26" s="65"/>
+      <c r="BF26" s="65"/>
+      <c r="BG26" s="65"/>
+      <c r="BH26" s="65"/>
+      <c r="BI26" s="65"/>
+      <c r="BJ26" s="65"/>
+      <c r="BK26" s="65"/>
+      <c r="BL26" s="65"/>
+      <c r="BM26" s="65"/>
+      <c r="BN26" s="65"/>
+      <c r="BO26" s="65"/>
+      <c r="BP26" s="65"/>
+      <c r="BQ26" s="65"/>
+      <c r="BR26" s="65"/>
+      <c r="BS26" s="65"/>
+      <c r="BT26" s="65"/>
+      <c r="BU26" s="65"/>
+      <c r="BV26" s="65"/>
+      <c r="BW26" s="65"/>
+      <c r="BX26" s="65"/>
+      <c r="BY26" s="65"/>
+      <c r="BZ26" s="65"/>
+      <c r="CA26" s="65"/>
+      <c r="CB26" s="65"/>
+      <c r="CC26" s="65"/>
+      <c r="CD26" s="65"/>
+      <c r="CE26" s="65"/>
+      <c r="CF26" s="65"/>
+      <c r="CG26" s="65"/>
+      <c r="CH26" s="65"/>
+      <c r="CI26" s="65"/>
+      <c r="CJ26" s="65"/>
+      <c r="CK26" s="65"/>
+      <c r="CL26" s="65"/>
+      <c r="CM26" s="65"/>
+      <c r="CN26" s="65"/>
+      <c r="CO26" s="65"/>
+      <c r="CP26" s="65"/>
+      <c r="CQ26" s="65"/>
+      <c r="CR26" s="65"/>
+      <c r="CS26" s="65"/>
+      <c r="CT26" s="65"/>
+      <c r="CU26" s="65"/>
+      <c r="CV26" s="65"/>
+      <c r="CW26" s="65"/>
+      <c r="CX26" s="65"/>
+      <c r="CY26" s="65"/>
+      <c r="CZ26" s="65"/>
+      <c r="DA26" s="65"/>
+      <c r="DB26" s="65"/>
+      <c r="DC26" s="65"/>
+      <c r="DD26" s="65"/>
+      <c r="DE26" s="65"/>
+      <c r="DF26" s="65"/>
+      <c r="DG26" s="65"/>
+      <c r="DH26" s="65"/>
+      <c r="DI26" s="65"/>
+      <c r="DJ26" s="65"/>
+      <c r="DK26" s="65"/>
+      <c r="DL26" s="65"/>
+      <c r="DM26" s="65"/>
+      <c r="DN26" s="65"/>
+      <c r="DO26" s="65"/>
+      <c r="DP26" s="65"/>
+      <c r="DQ26" s="65"/>
+      <c r="DR26" s="65"/>
+      <c r="DS26" s="65"/>
+      <c r="DT26" s="65"/>
+      <c r="DU26" s="65"/>
+      <c r="DV26" s="65"/>
+      <c r="DW26" s="65"/>
+      <c r="DX26" s="65"/>
+      <c r="DY26" s="65"/>
+      <c r="DZ26" s="65"/>
+      <c r="EA26" s="65"/>
+      <c r="EB26" s="65"/>
+      <c r="EC26" s="65"/>
+      <c r="ED26" s="65"/>
+      <c r="EE26" s="65"/>
+      <c r="EF26" s="65"/>
+      <c r="EG26" s="65"/>
+      <c r="EH26" s="65"/>
+      <c r="EI26" s="65"/>
+      <c r="EJ26" s="65"/>
+      <c r="EK26" s="65"/>
+      <c r="EL26" s="65"/>
+      <c r="EM26" s="65"/>
+      <c r="EN26" s="65"/>
+      <c r="EO26" s="65"/>
+      <c r="EP26" s="65"/>
+      <c r="EQ26" s="65"/>
+      <c r="ER26" s="65"/>
+      <c r="ES26" s="65"/>
+      <c r="ET26" s="65"/>
+      <c r="EU26" s="65"/>
+      <c r="EV26" s="65"/>
+      <c r="EW26" s="65"/>
+      <c r="EX26" s="65"/>
+      <c r="EY26" s="65"/>
+      <c r="EZ26" s="65"/>
+      <c r="FA26" s="65"/>
+      <c r="FB26" s="65"/>
+      <c r="FC26" s="65"/>
+      <c r="FD26" s="65"/>
+      <c r="FE26" s="65"/>
+      <c r="FF26" s="65"/>
+      <c r="FG26" s="65"/>
+      <c r="FH26" s="65"/>
+      <c r="FI26" s="65"/>
+      <c r="FJ26" s="65"/>
+      <c r="FK26" s="65"/>
+      <c r="FL26" s="65"/>
+      <c r="FM26" s="65"/>
+      <c r="FN26" s="65"/>
+      <c r="FO26" s="65"/>
+      <c r="FP26" s="65"/>
+      <c r="FQ26" s="65"/>
+      <c r="FR26" s="65"/>
+      <c r="FS26" s="65"/>
+      <c r="FT26" s="65"/>
+      <c r="FU26" s="65"/>
+      <c r="FV26" s="65"/>
+      <c r="FW26" s="65"/>
+      <c r="FX26" s="65"/>
+      <c r="FY26" s="65"/>
+      <c r="FZ26" s="65"/>
+      <c r="GA26" s="65"/>
+      <c r="GB26" s="65"/>
+      <c r="GC26" s="65"/>
+      <c r="GD26" s="65"/>
+      <c r="GE26" s="65"/>
+      <c r="GF26" s="65"/>
+      <c r="GG26" s="65"/>
+      <c r="GH26" s="65"/>
+      <c r="GI26" s="65"/>
+      <c r="GJ26" s="65"/>
+      <c r="GK26" s="65"/>
+      <c r="GL26" s="65"/>
+      <c r="GM26" s="65"/>
+      <c r="GN26" s="65"/>
+      <c r="GO26" s="65"/>
+      <c r="GP26" s="65"/>
+      <c r="GQ26" s="65"/>
+      <c r="GR26" s="65"/>
+      <c r="GS26" s="65"/>
+      <c r="GT26" s="65"/>
+      <c r="GU26" s="65"/>
+      <c r="GV26" s="65"/>
+      <c r="GW26" s="65"/>
+      <c r="GX26" s="65"/>
+      <c r="GY26" s="65"/>
+      <c r="GZ26" s="65"/>
+      <c r="HA26" s="65"/>
+      <c r="HB26" s="65"/>
+      <c r="HC26" s="65"/>
+      <c r="HD26" s="65"/>
+      <c r="HE26" s="65"/>
+      <c r="HF26" s="65"/>
+      <c r="HG26" s="65"/>
+      <c r="HH26" s="65"/>
+      <c r="HI26" s="65"/>
+      <c r="HJ26" s="65"/>
+      <c r="HK26" s="65"/>
+      <c r="HL26" s="65"/>
+      <c r="HM26" s="65"/>
+      <c r="HN26" s="65"/>
+      <c r="HO26" s="65"/>
+      <c r="HP26" s="65"/>
+      <c r="HQ26" s="65"/>
+      <c r="HR26" s="65"/>
+      <c r="HS26" s="65"/>
+      <c r="HT26" s="65"/>
+      <c r="HU26" s="65"/>
+      <c r="HV26" s="65"/>
+      <c r="HW26" s="65"/>
+      <c r="HX26" s="65"/>
+      <c r="HY26" s="65"/>
+      <c r="HZ26" s="65"/>
+      <c r="IA26" s="65"/>
+      <c r="IB26" s="65"/>
+      <c r="IC26" s="65"/>
+      <c r="ID26" s="65"/>
+      <c r="IE26" s="65"/>
+      <c r="IF26" s="65"/>
+      <c r="IG26" s="65"/>
+      <c r="IH26" s="65"/>
+      <c r="II26" s="65"/>
+      <c r="IJ26" s="65"/>
+      <c r="IK26" s="65"/>
+      <c r="IL26" s="65"/>
+      <c r="IM26" s="65"/>
+      <c r="IN26" s="65"/>
+      <c r="IO26" s="65"/>
+      <c r="IP26" s="65"/>
+      <c r="IQ26" s="65"/>
+      <c r="IR26" s="65"/>
+      <c r="IS26" s="65"/>
+      <c r="IT26" s="65"/>
+      <c r="IU26" s="65"/>
+      <c r="IV26" s="65"/>
+      <c r="IW26" s="65"/>
+      <c r="IX26" s="65"/>
+    </row>
+    <row r="27" spans="1:258" s="66" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A27" s="63"/>
+      <c r="B27" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="70"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="65"/>
+      <c r="U27" s="65"/>
+      <c r="V27" s="65"/>
+      <c r="W27" s="65"/>
+      <c r="X27" s="65"/>
+      <c r="Y27" s="65"/>
+      <c r="Z27" s="65"/>
+      <c r="AA27" s="65"/>
+      <c r="AB27" s="65"/>
+      <c r="AC27" s="65"/>
+      <c r="AD27" s="65"/>
+      <c r="AE27" s="65"/>
+      <c r="AF27" s="65"/>
+      <c r="AG27" s="65"/>
+      <c r="AH27" s="65"/>
+      <c r="AI27" s="65"/>
+      <c r="AJ27" s="65"/>
+      <c r="AK27" s="65"/>
+      <c r="AL27" s="65"/>
+      <c r="AM27" s="65"/>
+      <c r="AN27" s="65"/>
+      <c r="AO27" s="65"/>
+      <c r="AP27" s="65"/>
+      <c r="AQ27" s="65"/>
+      <c r="AR27" s="65"/>
+      <c r="AS27" s="65"/>
+      <c r="AT27" s="65"/>
+      <c r="AU27" s="65"/>
+      <c r="AV27" s="65"/>
+      <c r="AW27" s="65"/>
+      <c r="AX27" s="65"/>
+      <c r="AY27" s="65"/>
+      <c r="AZ27" s="65"/>
+      <c r="BA27" s="65"/>
+      <c r="BB27" s="65"/>
+      <c r="BC27" s="65"/>
+      <c r="BD27" s="65"/>
+      <c r="BE27" s="65"/>
+      <c r="BF27" s="65"/>
+      <c r="BG27" s="65"/>
+      <c r="BH27" s="65"/>
+      <c r="BI27" s="65"/>
+      <c r="BJ27" s="65"/>
+      <c r="BK27" s="65"/>
+      <c r="BL27" s="65"/>
+      <c r="BM27" s="65"/>
+      <c r="BN27" s="65"/>
+      <c r="BO27" s="65"/>
+      <c r="BP27" s="65"/>
+      <c r="BQ27" s="65"/>
+      <c r="BR27" s="65"/>
+      <c r="BS27" s="65"/>
+      <c r="BT27" s="65"/>
+      <c r="BU27" s="65"/>
+      <c r="BV27" s="65"/>
+      <c r="BW27" s="65"/>
+      <c r="BX27" s="65"/>
+      <c r="BY27" s="65"/>
+      <c r="BZ27" s="65"/>
+      <c r="CA27" s="65"/>
+      <c r="CB27" s="65"/>
+      <c r="CC27" s="65"/>
+      <c r="CD27" s="65"/>
+      <c r="CE27" s="65"/>
+      <c r="CF27" s="65"/>
+      <c r="CG27" s="65"/>
+      <c r="CH27" s="65"/>
+      <c r="CI27" s="65"/>
+      <c r="CJ27" s="65"/>
+      <c r="CK27" s="65"/>
+      <c r="CL27" s="65"/>
+      <c r="CM27" s="65"/>
+      <c r="CN27" s="65"/>
+      <c r="CO27" s="65"/>
+      <c r="CP27" s="65"/>
+      <c r="CQ27" s="65"/>
+      <c r="CR27" s="65"/>
+      <c r="CS27" s="65"/>
+      <c r="CT27" s="65"/>
+      <c r="CU27" s="65"/>
+      <c r="CV27" s="65"/>
+      <c r="CW27" s="65"/>
+      <c r="CX27" s="65"/>
+      <c r="CY27" s="65"/>
+      <c r="CZ27" s="65"/>
+      <c r="DA27" s="65"/>
+      <c r="DB27" s="65"/>
+      <c r="DC27" s="65"/>
+      <c r="DD27" s="65"/>
+      <c r="DE27" s="65"/>
+      <c r="DF27" s="65"/>
+      <c r="DG27" s="65"/>
+      <c r="DH27" s="65"/>
+      <c r="DI27" s="65"/>
+      <c r="DJ27" s="65"/>
+      <c r="DK27" s="65"/>
+      <c r="DL27" s="65"/>
+      <c r="DM27" s="65"/>
+      <c r="DN27" s="65"/>
+      <c r="DO27" s="65"/>
+      <c r="DP27" s="65"/>
+      <c r="DQ27" s="65"/>
+      <c r="DR27" s="65"/>
+      <c r="DS27" s="65"/>
+      <c r="DT27" s="65"/>
+      <c r="DU27" s="65"/>
+      <c r="DV27" s="65"/>
+      <c r="DW27" s="65"/>
+      <c r="DX27" s="65"/>
+      <c r="DY27" s="65"/>
+      <c r="DZ27" s="65"/>
+      <c r="EA27" s="65"/>
+      <c r="EB27" s="65"/>
+      <c r="EC27" s="65"/>
+      <c r="ED27" s="65"/>
+      <c r="EE27" s="65"/>
+      <c r="EF27" s="65"/>
+      <c r="EG27" s="65"/>
+      <c r="EH27" s="65"/>
+      <c r="EI27" s="65"/>
+      <c r="EJ27" s="65"/>
+      <c r="EK27" s="65"/>
+      <c r="EL27" s="65"/>
+      <c r="EM27" s="65"/>
+      <c r="EN27" s="65"/>
+      <c r="EO27" s="65"/>
+      <c r="EP27" s="65"/>
+      <c r="EQ27" s="65"/>
+      <c r="ER27" s="65"/>
+      <c r="ES27" s="65"/>
+      <c r="ET27" s="65"/>
+      <c r="EU27" s="65"/>
+      <c r="EV27" s="65"/>
+      <c r="EW27" s="65"/>
+      <c r="EX27" s="65"/>
+      <c r="EY27" s="65"/>
+      <c r="EZ27" s="65"/>
+      <c r="FA27" s="65"/>
+      <c r="FB27" s="65"/>
+      <c r="FC27" s="65"/>
+      <c r="FD27" s="65"/>
+      <c r="FE27" s="65"/>
+      <c r="FF27" s="65"/>
+      <c r="FG27" s="65"/>
+      <c r="FH27" s="65"/>
+      <c r="FI27" s="65"/>
+      <c r="FJ27" s="65"/>
+      <c r="FK27" s="65"/>
+      <c r="FL27" s="65"/>
+      <c r="FM27" s="65"/>
+      <c r="FN27" s="65"/>
+      <c r="FO27" s="65"/>
+      <c r="FP27" s="65"/>
+      <c r="FQ27" s="65"/>
+      <c r="FR27" s="65"/>
+      <c r="FS27" s="65"/>
+      <c r="FT27" s="65"/>
+      <c r="FU27" s="65"/>
+      <c r="FV27" s="65"/>
+      <c r="FW27" s="65"/>
+      <c r="FX27" s="65"/>
+      <c r="FY27" s="65"/>
+      <c r="FZ27" s="65"/>
+      <c r="GA27" s="65"/>
+      <c r="GB27" s="65"/>
+      <c r="GC27" s="65"/>
+      <c r="GD27" s="65"/>
+      <c r="GE27" s="65"/>
+      <c r="GF27" s="65"/>
+      <c r="GG27" s="65"/>
+      <c r="GH27" s="65"/>
+      <c r="GI27" s="65"/>
+      <c r="GJ27" s="65"/>
+      <c r="GK27" s="65"/>
+      <c r="GL27" s="65"/>
+      <c r="GM27" s="65"/>
+      <c r="GN27" s="65"/>
+      <c r="GO27" s="65"/>
+      <c r="GP27" s="65"/>
+      <c r="GQ27" s="65"/>
+      <c r="GR27" s="65"/>
+      <c r="GS27" s="65"/>
+      <c r="GT27" s="65"/>
+      <c r="GU27" s="65"/>
+      <c r="GV27" s="65"/>
+      <c r="GW27" s="65"/>
+      <c r="GX27" s="65"/>
+      <c r="GY27" s="65"/>
+      <c r="GZ27" s="65"/>
+      <c r="HA27" s="65"/>
+      <c r="HB27" s="65"/>
+      <c r="HC27" s="65"/>
+      <c r="HD27" s="65"/>
+      <c r="HE27" s="65"/>
+      <c r="HF27" s="65"/>
+      <c r="HG27" s="65"/>
+      <c r="HH27" s="65"/>
+      <c r="HI27" s="65"/>
+      <c r="HJ27" s="65"/>
+      <c r="HK27" s="65"/>
+      <c r="HL27" s="65"/>
+      <c r="HM27" s="65"/>
+      <c r="HN27" s="65"/>
+      <c r="HO27" s="65"/>
+      <c r="HP27" s="65"/>
+      <c r="HQ27" s="65"/>
+      <c r="HR27" s="65"/>
+      <c r="HS27" s="65"/>
+      <c r="HT27" s="65"/>
+      <c r="HU27" s="65"/>
+      <c r="HV27" s="65"/>
+      <c r="HW27" s="65"/>
+      <c r="HX27" s="65"/>
+      <c r="HY27" s="65"/>
+      <c r="HZ27" s="65"/>
+      <c r="IA27" s="65"/>
+      <c r="IB27" s="65"/>
+      <c r="IC27" s="65"/>
+      <c r="ID27" s="65"/>
+      <c r="IE27" s="65"/>
+      <c r="IF27" s="65"/>
+      <c r="IG27" s="65"/>
+      <c r="IH27" s="65"/>
+      <c r="II27" s="65"/>
+      <c r="IJ27" s="65"/>
+      <c r="IK27" s="65"/>
+      <c r="IL27" s="65"/>
+      <c r="IM27" s="65"/>
+      <c r="IN27" s="65"/>
+      <c r="IO27" s="65"/>
+      <c r="IP27" s="65"/>
+      <c r="IQ27" s="65"/>
+      <c r="IR27" s="65"/>
+      <c r="IS27" s="65"/>
+      <c r="IT27" s="65"/>
+      <c r="IU27" s="65"/>
+      <c r="IV27" s="65"/>
+      <c r="IW27" s="65"/>
+      <c r="IX27" s="65"/>
+    </row>
+    <row r="28" spans="1:258" s="66" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A28" s="63"/>
+      <c r="B28" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="71"/>
+      <c r="D28" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" s="70"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="65"/>
+      <c r="Y28" s="65"/>
+      <c r="Z28" s="65"/>
+      <c r="AA28" s="65"/>
+      <c r="AB28" s="65"/>
+      <c r="AC28" s="65"/>
+      <c r="AD28" s="65"/>
+      <c r="AE28" s="65"/>
+      <c r="AF28" s="65"/>
+      <c r="AG28" s="65"/>
+      <c r="AH28" s="65"/>
+      <c r="AI28" s="65"/>
+      <c r="AJ28" s="65"/>
+      <c r="AK28" s="65"/>
+      <c r="AL28" s="65"/>
+      <c r="AM28" s="65"/>
+      <c r="AN28" s="65"/>
+      <c r="AO28" s="65"/>
+      <c r="AP28" s="65"/>
+      <c r="AQ28" s="65"/>
+      <c r="AR28" s="65"/>
+      <c r="AS28" s="65"/>
+      <c r="AT28" s="65"/>
+      <c r="AU28" s="65"/>
+      <c r="AV28" s="65"/>
+      <c r="AW28" s="65"/>
+      <c r="AX28" s="65"/>
+      <c r="AY28" s="65"/>
+      <c r="AZ28" s="65"/>
+      <c r="BA28" s="65"/>
+      <c r="BB28" s="65"/>
+      <c r="BC28" s="65"/>
+      <c r="BD28" s="65"/>
+      <c r="BE28" s="65"/>
+      <c r="BF28" s="65"/>
+      <c r="BG28" s="65"/>
+      <c r="BH28" s="65"/>
+      <c r="BI28" s="65"/>
+      <c r="BJ28" s="65"/>
+      <c r="BK28" s="65"/>
+      <c r="BL28" s="65"/>
+      <c r="BM28" s="65"/>
+      <c r="BN28" s="65"/>
+      <c r="BO28" s="65"/>
+      <c r="BP28" s="65"/>
+      <c r="BQ28" s="65"/>
+      <c r="BR28" s="65"/>
+      <c r="BS28" s="65"/>
+      <c r="BT28" s="65"/>
+      <c r="BU28" s="65"/>
+      <c r="BV28" s="65"/>
+      <c r="BW28" s="65"/>
+      <c r="BX28" s="65"/>
+      <c r="BY28" s="65"/>
+      <c r="BZ28" s="65"/>
+      <c r="CA28" s="65"/>
+      <c r="CB28" s="65"/>
+      <c r="CC28" s="65"/>
+      <c r="CD28" s="65"/>
+      <c r="CE28" s="65"/>
+      <c r="CF28" s="65"/>
+      <c r="CG28" s="65"/>
+      <c r="CH28" s="65"/>
+      <c r="CI28" s="65"/>
+      <c r="CJ28" s="65"/>
+      <c r="CK28" s="65"/>
+      <c r="CL28" s="65"/>
+      <c r="CM28" s="65"/>
+      <c r="CN28" s="65"/>
+      <c r="CO28" s="65"/>
+      <c r="CP28" s="65"/>
+      <c r="CQ28" s="65"/>
+      <c r="CR28" s="65"/>
+      <c r="CS28" s="65"/>
+      <c r="CT28" s="65"/>
+      <c r="CU28" s="65"/>
+      <c r="CV28" s="65"/>
+      <c r="CW28" s="65"/>
+      <c r="CX28" s="65"/>
+      <c r="CY28" s="65"/>
+      <c r="CZ28" s="65"/>
+      <c r="DA28" s="65"/>
+      <c r="DB28" s="65"/>
+      <c r="DC28" s="65"/>
+      <c r="DD28" s="65"/>
+      <c r="DE28" s="65"/>
+      <c r="DF28" s="65"/>
+      <c r="DG28" s="65"/>
+      <c r="DH28" s="65"/>
+      <c r="DI28" s="65"/>
+      <c r="DJ28" s="65"/>
+      <c r="DK28" s="65"/>
+      <c r="DL28" s="65"/>
+      <c r="DM28" s="65"/>
+      <c r="DN28" s="65"/>
+      <c r="DO28" s="65"/>
+      <c r="DP28" s="65"/>
+      <c r="DQ28" s="65"/>
+      <c r="DR28" s="65"/>
+      <c r="DS28" s="65"/>
+      <c r="DT28" s="65"/>
+      <c r="DU28" s="65"/>
+      <c r="DV28" s="65"/>
+      <c r="DW28" s="65"/>
+      <c r="DX28" s="65"/>
+      <c r="DY28" s="65"/>
+      <c r="DZ28" s="65"/>
+      <c r="EA28" s="65"/>
+      <c r="EB28" s="65"/>
+      <c r="EC28" s="65"/>
+      <c r="ED28" s="65"/>
+      <c r="EE28" s="65"/>
+      <c r="EF28" s="65"/>
+      <c r="EG28" s="65"/>
+      <c r="EH28" s="65"/>
+      <c r="EI28" s="65"/>
+      <c r="EJ28" s="65"/>
+      <c r="EK28" s="65"/>
+      <c r="EL28" s="65"/>
+      <c r="EM28" s="65"/>
+      <c r="EN28" s="65"/>
+      <c r="EO28" s="65"/>
+      <c r="EP28" s="65"/>
+      <c r="EQ28" s="65"/>
+      <c r="ER28" s="65"/>
+      <c r="ES28" s="65"/>
+      <c r="ET28" s="65"/>
+      <c r="EU28" s="65"/>
+      <c r="EV28" s="65"/>
+      <c r="EW28" s="65"/>
+      <c r="EX28" s="65"/>
+      <c r="EY28" s="65"/>
+      <c r="EZ28" s="65"/>
+      <c r="FA28" s="65"/>
+      <c r="FB28" s="65"/>
+      <c r="FC28" s="65"/>
+      <c r="FD28" s="65"/>
+      <c r="FE28" s="65"/>
+      <c r="FF28" s="65"/>
+      <c r="FG28" s="65"/>
+      <c r="FH28" s="65"/>
+      <c r="FI28" s="65"/>
+      <c r="FJ28" s="65"/>
+      <c r="FK28" s="65"/>
+      <c r="FL28" s="65"/>
+      <c r="FM28" s="65"/>
+      <c r="FN28" s="65"/>
+      <c r="FO28" s="65"/>
+      <c r="FP28" s="65"/>
+      <c r="FQ28" s="65"/>
+      <c r="FR28" s="65"/>
+      <c r="FS28" s="65"/>
+      <c r="FT28" s="65"/>
+      <c r="FU28" s="65"/>
+      <c r="FV28" s="65"/>
+      <c r="FW28" s="65"/>
+      <c r="FX28" s="65"/>
+      <c r="FY28" s="65"/>
+      <c r="FZ28" s="65"/>
+      <c r="GA28" s="65"/>
+      <c r="GB28" s="65"/>
+      <c r="GC28" s="65"/>
+      <c r="GD28" s="65"/>
+      <c r="GE28" s="65"/>
+      <c r="GF28" s="65"/>
+      <c r="GG28" s="65"/>
+      <c r="GH28" s="65"/>
+      <c r="GI28" s="65"/>
+      <c r="GJ28" s="65"/>
+      <c r="GK28" s="65"/>
+      <c r="GL28" s="65"/>
+      <c r="GM28" s="65"/>
+      <c r="GN28" s="65"/>
+      <c r="GO28" s="65"/>
+      <c r="GP28" s="65"/>
+      <c r="GQ28" s="65"/>
+      <c r="GR28" s="65"/>
+      <c r="GS28" s="65"/>
+      <c r="GT28" s="65"/>
+      <c r="GU28" s="65"/>
+      <c r="GV28" s="65"/>
+      <c r="GW28" s="65"/>
+      <c r="GX28" s="65"/>
+      <c r="GY28" s="65"/>
+      <c r="GZ28" s="65"/>
+      <c r="HA28" s="65"/>
+      <c r="HB28" s="65"/>
+      <c r="HC28" s="65"/>
+      <c r="HD28" s="65"/>
+      <c r="HE28" s="65"/>
+      <c r="HF28" s="65"/>
+      <c r="HG28" s="65"/>
+      <c r="HH28" s="65"/>
+      <c r="HI28" s="65"/>
+      <c r="HJ28" s="65"/>
+      <c r="HK28" s="65"/>
+      <c r="HL28" s="65"/>
+      <c r="HM28" s="65"/>
+      <c r="HN28" s="65"/>
+      <c r="HO28" s="65"/>
+      <c r="HP28" s="65"/>
+      <c r="HQ28" s="65"/>
+      <c r="HR28" s="65"/>
+      <c r="HS28" s="65"/>
+      <c r="HT28" s="65"/>
+      <c r="HU28" s="65"/>
+      <c r="HV28" s="65"/>
+      <c r="HW28" s="65"/>
+      <c r="HX28" s="65"/>
+      <c r="HY28" s="65"/>
+      <c r="HZ28" s="65"/>
+      <c r="IA28" s="65"/>
+      <c r="IB28" s="65"/>
+      <c r="IC28" s="65"/>
+      <c r="ID28" s="65"/>
+      <c r="IE28" s="65"/>
+      <c r="IF28" s="65"/>
+      <c r="IG28" s="65"/>
+      <c r="IH28" s="65"/>
+      <c r="II28" s="65"/>
+      <c r="IJ28" s="65"/>
+      <c r="IK28" s="65"/>
+      <c r="IL28" s="65"/>
+      <c r="IM28" s="65"/>
+      <c r="IN28" s="65"/>
+      <c r="IO28" s="65"/>
+      <c r="IP28" s="65"/>
+      <c r="IQ28" s="65"/>
+      <c r="IR28" s="65"/>
+      <c r="IS28" s="65"/>
+      <c r="IT28" s="65"/>
+      <c r="IU28" s="65"/>
+      <c r="IV28" s="65"/>
+      <c r="IW28" s="65"/>
+      <c r="IX28" s="65"/>
+    </row>
+    <row r="29" spans="1:258" s="66" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A29" s="63"/>
+      <c r="B29" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="68"/>
+      <c r="D29" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="70"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="65"/>
+      <c r="O29" s="65"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="65"/>
+      <c r="R29" s="65"/>
+      <c r="S29" s="65"/>
+      <c r="T29" s="65"/>
+      <c r="U29" s="65"/>
+      <c r="V29" s="65"/>
+      <c r="W29" s="65"/>
+      <c r="X29" s="65"/>
+      <c r="Y29" s="65"/>
+      <c r="Z29" s="65"/>
+      <c r="AA29" s="65"/>
+      <c r="AB29" s="65"/>
+      <c r="AC29" s="65"/>
+      <c r="AD29" s="65"/>
+      <c r="AE29" s="65"/>
+      <c r="AF29" s="65"/>
+      <c r="AG29" s="65"/>
+      <c r="AH29" s="65"/>
+      <c r="AI29" s="65"/>
+      <c r="AJ29" s="65"/>
+      <c r="AK29" s="65"/>
+      <c r="AL29" s="65"/>
+      <c r="AM29" s="65"/>
+      <c r="AN29" s="65"/>
+      <c r="AO29" s="65"/>
+      <c r="AP29" s="65"/>
+      <c r="AQ29" s="65"/>
+      <c r="AR29" s="65"/>
+      <c r="AS29" s="65"/>
+      <c r="AT29" s="65"/>
+      <c r="AU29" s="65"/>
+      <c r="AV29" s="65"/>
+      <c r="AW29" s="65"/>
+      <c r="AX29" s="65"/>
+      <c r="AY29" s="65"/>
+      <c r="AZ29" s="65"/>
+      <c r="BA29" s="65"/>
+      <c r="BB29" s="65"/>
+      <c r="BC29" s="65"/>
+      <c r="BD29" s="65"/>
+      <c r="BE29" s="65"/>
+      <c r="BF29" s="65"/>
+      <c r="BG29" s="65"/>
+      <c r="BH29" s="65"/>
+      <c r="BI29" s="65"/>
+      <c r="BJ29" s="65"/>
+      <c r="BK29" s="65"/>
+      <c r="BL29" s="65"/>
+      <c r="BM29" s="65"/>
+      <c r="BN29" s="65"/>
+      <c r="BO29" s="65"/>
+      <c r="BP29" s="65"/>
+      <c r="BQ29" s="65"/>
+      <c r="BR29" s="65"/>
+      <c r="BS29" s="65"/>
+      <c r="BT29" s="65"/>
+      <c r="BU29" s="65"/>
+      <c r="BV29" s="65"/>
+      <c r="BW29" s="65"/>
+      <c r="BX29" s="65"/>
+      <c r="BY29" s="65"/>
+      <c r="BZ29" s="65"/>
+      <c r="CA29" s="65"/>
+      <c r="CB29" s="65"/>
+      <c r="CC29" s="65"/>
+      <c r="CD29" s="65"/>
+      <c r="CE29" s="65"/>
+      <c r="CF29" s="65"/>
+      <c r="CG29" s="65"/>
+      <c r="CH29" s="65"/>
+      <c r="CI29" s="65"/>
+      <c r="CJ29" s="65"/>
+      <c r="CK29" s="65"/>
+      <c r="CL29" s="65"/>
+      <c r="CM29" s="65"/>
+      <c r="CN29" s="65"/>
+      <c r="CO29" s="65"/>
+      <c r="CP29" s="65"/>
+      <c r="CQ29" s="65"/>
+      <c r="CR29" s="65"/>
+      <c r="CS29" s="65"/>
+      <c r="CT29" s="65"/>
+      <c r="CU29" s="65"/>
+      <c r="CV29" s="65"/>
+      <c r="CW29" s="65"/>
+      <c r="CX29" s="65"/>
+      <c r="CY29" s="65"/>
+      <c r="CZ29" s="65"/>
+      <c r="DA29" s="65"/>
+      <c r="DB29" s="65"/>
+      <c r="DC29" s="65"/>
+      <c r="DD29" s="65"/>
+      <c r="DE29" s="65"/>
+      <c r="DF29" s="65"/>
+      <c r="DG29" s="65"/>
+      <c r="DH29" s="65"/>
+      <c r="DI29" s="65"/>
+      <c r="DJ29" s="65"/>
+      <c r="DK29" s="65"/>
+      <c r="DL29" s="65"/>
+      <c r="DM29" s="65"/>
+      <c r="DN29" s="65"/>
+      <c r="DO29" s="65"/>
+      <c r="DP29" s="65"/>
+      <c r="DQ29" s="65"/>
+      <c r="DR29" s="65"/>
+      <c r="DS29" s="65"/>
+      <c r="DT29" s="65"/>
+      <c r="DU29" s="65"/>
+      <c r="DV29" s="65"/>
+      <c r="DW29" s="65"/>
+      <c r="DX29" s="65"/>
+      <c r="DY29" s="65"/>
+      <c r="DZ29" s="65"/>
+      <c r="EA29" s="65"/>
+      <c r="EB29" s="65"/>
+      <c r="EC29" s="65"/>
+      <c r="ED29" s="65"/>
+      <c r="EE29" s="65"/>
+      <c r="EF29" s="65"/>
+      <c r="EG29" s="65"/>
+      <c r="EH29" s="65"/>
+      <c r="EI29" s="65"/>
+      <c r="EJ29" s="65"/>
+      <c r="EK29" s="65"/>
+      <c r="EL29" s="65"/>
+      <c r="EM29" s="65"/>
+      <c r="EN29" s="65"/>
+      <c r="EO29" s="65"/>
+      <c r="EP29" s="65"/>
+      <c r="EQ29" s="65"/>
+      <c r="ER29" s="65"/>
+      <c r="ES29" s="65"/>
+      <c r="ET29" s="65"/>
+      <c r="EU29" s="65"/>
+      <c r="EV29" s="65"/>
+      <c r="EW29" s="65"/>
+      <c r="EX29" s="65"/>
+      <c r="EY29" s="65"/>
+      <c r="EZ29" s="65"/>
+      <c r="FA29" s="65"/>
+      <c r="FB29" s="65"/>
+      <c r="FC29" s="65"/>
+      <c r="FD29" s="65"/>
+      <c r="FE29" s="65"/>
+      <c r="FF29" s="65"/>
+      <c r="FG29" s="65"/>
+      <c r="FH29" s="65"/>
+      <c r="FI29" s="65"/>
+      <c r="FJ29" s="65"/>
+      <c r="FK29" s="65"/>
+      <c r="FL29" s="65"/>
+      <c r="FM29" s="65"/>
+      <c r="FN29" s="65"/>
+      <c r="FO29" s="65"/>
+      <c r="FP29" s="65"/>
+      <c r="FQ29" s="65"/>
+      <c r="FR29" s="65"/>
+      <c r="FS29" s="65"/>
+      <c r="FT29" s="65"/>
+      <c r="FU29" s="65"/>
+      <c r="FV29" s="65"/>
+      <c r="FW29" s="65"/>
+      <c r="FX29" s="65"/>
+      <c r="FY29" s="65"/>
+      <c r="FZ29" s="65"/>
+      <c r="GA29" s="65"/>
+      <c r="GB29" s="65"/>
+      <c r="GC29" s="65"/>
+      <c r="GD29" s="65"/>
+      <c r="GE29" s="65"/>
+      <c r="GF29" s="65"/>
+      <c r="GG29" s="65"/>
+      <c r="GH29" s="65"/>
+      <c r="GI29" s="65"/>
+      <c r="GJ29" s="65"/>
+      <c r="GK29" s="65"/>
+      <c r="GL29" s="65"/>
+      <c r="GM29" s="65"/>
+      <c r="GN29" s="65"/>
+      <c r="GO29" s="65"/>
+      <c r="GP29" s="65"/>
+      <c r="GQ29" s="65"/>
+      <c r="GR29" s="65"/>
+      <c r="GS29" s="65"/>
+      <c r="GT29" s="65"/>
+      <c r="GU29" s="65"/>
+      <c r="GV29" s="65"/>
+      <c r="GW29" s="65"/>
+      <c r="GX29" s="65"/>
+      <c r="GY29" s="65"/>
+      <c r="GZ29" s="65"/>
+      <c r="HA29" s="65"/>
+      <c r="HB29" s="65"/>
+      <c r="HC29" s="65"/>
+      <c r="HD29" s="65"/>
+      <c r="HE29" s="65"/>
+      <c r="HF29" s="65"/>
+      <c r="HG29" s="65"/>
+      <c r="HH29" s="65"/>
+      <c r="HI29" s="65"/>
+      <c r="HJ29" s="65"/>
+      <c r="HK29" s="65"/>
+      <c r="HL29" s="65"/>
+      <c r="HM29" s="65"/>
+      <c r="HN29" s="65"/>
+      <c r="HO29" s="65"/>
+      <c r="HP29" s="65"/>
+      <c r="HQ29" s="65"/>
+      <c r="HR29" s="65"/>
+      <c r="HS29" s="65"/>
+      <c r="HT29" s="65"/>
+      <c r="HU29" s="65"/>
+      <c r="HV29" s="65"/>
+      <c r="HW29" s="65"/>
+      <c r="HX29" s="65"/>
+      <c r="HY29" s="65"/>
+      <c r="HZ29" s="65"/>
+      <c r="IA29" s="65"/>
+      <c r="IB29" s="65"/>
+      <c r="IC29" s="65"/>
+      <c r="ID29" s="65"/>
+      <c r="IE29" s="65"/>
+      <c r="IF29" s="65"/>
+      <c r="IG29" s="65"/>
+      <c r="IH29" s="65"/>
+      <c r="II29" s="65"/>
+      <c r="IJ29" s="65"/>
+      <c r="IK29" s="65"/>
+      <c r="IL29" s="65"/>
+      <c r="IM29" s="65"/>
+      <c r="IN29" s="65"/>
+      <c r="IO29" s="65"/>
+      <c r="IP29" s="65"/>
+      <c r="IQ29" s="65"/>
+      <c r="IR29" s="65"/>
+      <c r="IS29" s="65"/>
+      <c r="IT29" s="65"/>
+      <c r="IU29" s="65"/>
+      <c r="IV29" s="65"/>
+      <c r="IW29" s="65"/>
+      <c r="IX29" s="65"/>
+    </row>
+    <row r="30" spans="1:258" ht="19.899999999999999" customHeight="1" thickBot="1">
+      <c r="B30" s="37"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="38"/>
+    </row>
+    <row r="31" spans="1:258" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B31" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-    </row>
-    <row r="28" spans="1:258" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="B28" s="56" t="s">
+      <c r="C31" s="74"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+    </row>
+    <row r="32" spans="1:258" ht="19.899999999999999" customHeight="1" thickTop="1">
+      <c r="B32" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C32" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="57" t="s">
+      <c r="D32" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E32" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="57" t="s">
+      <c r="F32" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="58" t="s">
+      <c r="G32" s="43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:258" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="59">
+    <row r="33" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B33" s="44">
         <v>1</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C33" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
-    </row>
-    <row r="30" spans="1:258" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="59">
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
+    </row>
+    <row r="34" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B34" s="44">
         <v>2</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="62"/>
-    </row>
-    <row r="31" spans="1:258" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="59">
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
+    </row>
+    <row r="35" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B35" s="44">
         <v>3</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C35" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="62"/>
-    </row>
-    <row r="32" spans="1:258" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="59">
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
+    </row>
+    <row r="36" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B36" s="44">
         <v>4</v>
       </c>
-      <c r="C32" s="63" t="s">
+      <c r="C36" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="62"/>
-    </row>
-    <row r="33" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="B33" s="59">
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="47"/>
+    </row>
+    <row r="37" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B37" s="44">
         <v>5</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C37" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="62"/>
-    </row>
-    <row r="34" spans="1:9" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="B34" s="64">
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="47"/>
+    </row>
+    <row r="38" spans="1:9" ht="19.899999999999999" customHeight="1" thickBot="1">
+      <c r="B38" s="49">
         <v>6</v>
       </c>
-      <c r="C34" s="65" t="s">
+      <c r="C38" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="67"/>
-    </row>
-    <row r="35" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1"/>
-    <row r="36" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B36" s="69" t="s">
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="52"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1"/>
+    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B40" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="69"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-    </row>
-    <row r="37" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="B37" s="56" t="s">
+      <c r="C40" s="74"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+    </row>
+    <row r="41" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1">
+      <c r="B41" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C41" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="57" t="s">
+      <c r="D41" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="57" t="s">
+      <c r="E41" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="57" t="s">
+      <c r="F41" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="58" t="s">
+      <c r="G41" s="43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="B38" s="59">
+    <row r="42" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B42" s="44">
         <v>1</v>
       </c>
-      <c r="C38" s="60" t="s">
+      <c r="C42" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="62"/>
-    </row>
-    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="B39" s="59">
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
+    </row>
+    <row r="43" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B43" s="44">
         <v>2</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C43" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="62"/>
-      <c r="I39"/>
-    </row>
-    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="B40" s="59">
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B44" s="44">
         <v>3</v>
       </c>
-      <c r="C40" s="63" t="s">
+      <c r="C44" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="62"/>
-    </row>
-    <row r="41" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="B41" s="59">
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="47"/>
+    </row>
+    <row r="45" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B45" s="44">
         <v>4</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C45" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="62"/>
-    </row>
-    <row r="42" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="B42" s="59">
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="47"/>
+    </row>
+    <row r="46" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="B46" s="44">
         <v>5</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C46" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="62"/>
-    </row>
-    <row r="43" spans="1:9" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="B43" s="64">
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="47"/>
+    </row>
+    <row r="47" spans="1:9" ht="19.899999999999999" customHeight="1" thickBot="1">
+      <c r="B47" s="49">
         <v>6</v>
       </c>
-      <c r="C43" s="65" t="s">
+      <c r="C47" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="67"/>
-    </row>
-    <row r="44" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-    </row>
-    <row r="45" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-    </row>
-    <row r="46" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="A46" s="30"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-    </row>
-    <row r="47" spans="1:9" ht="19.899999999999999" customHeight="1">
-      <c r="A47" s="30"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-    </row>
-    <row r="48" spans="1:9" ht="19.899999999999999" customHeight="1">
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="52"/>
+    </row>
+    <row r="48" spans="1:9" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A48" s="30"/>
       <c r="B48" s="35"/>
       <c r="C48" s="25"/>
@@ -3296,7 +4383,9 @@
     </row>
     <row r="49" spans="1:5" ht="19.899999999999999" customHeight="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="25"/>
+      <c r="B49" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
@@ -3323,24 +4412,28 @@
       <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:5" ht="19.899999999999999" customHeight="1">
+      <c r="A53" s="30"/>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:5" ht="19.899999999999999" customHeight="1">
+      <c r="A54" s="30"/>
       <c r="B54" s="35"/>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
       <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:5" ht="19.899999999999999" customHeight="1">
+      <c r="A55" s="30"/>
       <c r="B55" s="25"/>
       <c r="C55" s="25"/>
       <c r="D55" s="25"/>
       <c r="E55" s="25"/>
     </row>
     <row r="56" spans="1:5" ht="19.899999999999999" customHeight="1">
+      <c r="A56" s="30"/>
       <c r="B56" s="35"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
@@ -3352,25 +4445,25 @@
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" ht="19.899999999999999" customHeight="1">
       <c r="B58" s="35"/>
       <c r="C58" s="25"/>
       <c r="D58" s="25"/>
       <c r="E58" s="25"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" ht="19.899999999999999" customHeight="1">
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25"/>
       <c r="E59" s="25"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" ht="19.899999999999999" customHeight="1">
       <c r="B60" s="35"/>
       <c r="C60" s="25"/>
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" ht="19.899999999999999" customHeight="1">
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -3395,18 +4488,67 @@
       <c r="E64" s="25"/>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="27"/>
+      <c r="B65" s="25"/>
       <c r="C65" s="25"/>
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
     </row>
     <row r="66" spans="2:5">
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
       <c r="E66" s="25"/>
     </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="35"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="27"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="33">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B13:G15"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F20:G20"/>
@@ -3415,23 +4557,6 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B13:G15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.9763779527559058E-2" bottom="3.9763779527559058E-2" header="0" footer="0"/>
@@ -3444,7 +4569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IV89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
@@ -3466,45 +4591,45 @@
       <c r="F2"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
     </row>
     <row r="7" spans="2:8" ht="30">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="78"/>
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
     </row>
     <row r="12" spans="2:8">
       <c r="F12" s="3"/>
     </row>
     <row r="15" spans="2:8" ht="30">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickBot="1">
       <c r="B17"/>
@@ -3515,54 +4640,54 @@
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
     </row>
     <row r="19" spans="2:16" ht="18">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
     </row>
     <row r="20" spans="2:16" ht="18">
       <c r="B20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
     </row>
     <row r="21" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
     </row>
     <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="43"/>
+      <c r="D22" s="92"/>
       <c r="E22" s="8" t="s">
         <v>12</v>
       </c>
@@ -3574,8 +4699,8 @@
       <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
       <c r="E23" s="10" t="s">
         <v>15</v>
       </c>
@@ -3585,8 +4710,8 @@
     </row>
     <row r="24" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B24" s="11"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
       <c r="E24" s="13" t="s">
         <v>16</v>
       </c>
@@ -3616,10 +4741,10 @@
       <c r="C28" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="46"/>
+      <c r="E28" s="88"/>
       <c r="F28" s="19" t="s">
         <v>23</v>
       </c>
@@ -3631,10 +4756,10 @@
       <c r="C29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="47"/>
+      <c r="E29" s="89"/>
       <c r="F29" s="22" t="s">
         <v>13</v>
       </c>
@@ -3642,57 +4767,57 @@
     <row r="30" spans="2:16" ht="25.5" customHeight="1">
       <c r="B30" s="23"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="2:16" ht="25.5" customHeight="1">
       <c r="B31" s="23"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="85"/>
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="2:16" ht="25.5" customHeight="1">
       <c r="B32" s="23"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="85"/>
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:10" ht="25.5" customHeight="1">
       <c r="B33" s="23"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:10" ht="25.5" customHeight="1">
       <c r="B34" s="23"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:10" ht="25.5" customHeight="1">
       <c r="B35" s="23"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
       <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:10" ht="25.5" customHeight="1">
       <c r="B36" s="23"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:10" ht="25.5" customHeight="1" thickBot="1">
       <c r="B37" s="24"/>
       <c r="C37" s="12"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
       <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -3706,52 +4831,52 @@
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" thickBot="1"/>
     <row r="41" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
     </row>
     <row r="42" spans="1:10" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
     </row>
     <row r="43" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="83"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="83"/>
+      <c r="F43" s="83"/>
       <c r="J43" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
+      <c r="B44" s="83"/>
+      <c r="C44" s="83"/>
+      <c r="D44" s="83"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
       <c r="G45" s="25"/>
     </row>
     <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="84"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="84"/>
     </row>
     <row r="47" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A47" s="26"/>
@@ -4067,16 +5192,18 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="D28:E28"/>
@@ -4084,18 +5211,16 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.9763779527559058E-2" bottom="3.9763779527559058E-2" header="0" footer="0"/>

</xml_diff>